<commit_message>
fill with product backlog
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -662,6 +662,144 @@
   </si>
   <si>
     <t xml:space="preserve">L.W 03/15/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Helper, I want to check out and fund all selected needs in my funding basket so that my contributions are submitted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I have selected needs in my funding basket when I proceed to checkout then I expect to see a summary of the selected needs and their total cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I am ready to fund the selected needs when I confirm the checkout then I expect my contributions to be submitted successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I have insufficient funds when I try to check out then I expect to see an error message indicating insufficient funds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a U-fund Manager, I want to be able to search for needs so I can find a specific need quickly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIVEN I submit a request to search for a specific need in my cupboard WHEN there is a need that contains that text, THEN the system should return a list of needs containing only needs that contain the text and a status code of OK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIVEN I submit a request to search for a specific need in my cupboard WHEN there are no needs that contains that text, THEN the system should return an empty list and a status code of OK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**NOT IMPLEMENTED YET** As a Helper, I want to be able to save needs to a wish list so I can revisit needs that I have interest in in the future.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As a Helper, I want to remove needs from my wish list in case I will not be able to afford them in the future.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am logged in as a helper when I click remove on a need in my wishlist then the need will be removed from my wishlist.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As a Helper, I want to view my wish list so I can see the needs I have saved for purchasing later</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I have items in my wish list when I view my wish list then I expect to see a list of all the needs I have saved for later</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that my wish list is empty when I view it then I expect to see a message indicating that the wish list is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I have items in my wish list when I remove an item then I expect that item to be removed from the wish list</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As a Helper, I would like to filter my searches based on whether or not I’ve viewed them before so I can browse needs I have not seen.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">given that there are both viewed and unviewed needs when I filter for unviewed needs then I expect to see only needs I have not seen before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that there are only viewed needs when I filter for unviewed needs then I expect to see a "no results found" message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I reset the filters when I clear the viewed/unviewed filter then I expect to see all available needs again</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">As a Helper, I would like to filter my searches by price so I can view needs within my current budget.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">given that needs exist with different prices when I filter by a specific price range then I expect to see only the needs within that range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that no needs exist within the selected price range when I filter by that range then I expect to see a "no results found" message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">given that I reset the filters when I clear the price filter then I expect to see all available needs again</t>
   </si>
 </sst>
 </file>
@@ -671,7 +809,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -732,6 +870,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -782,7 +926,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -833,6 +977,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1172,10 +1324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F591"/>
+  <dimension ref="A1:F595"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.87890625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1411,67 +1563,137 @@
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="C19" s="10"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C20" s="10"/>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C21" s="10"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C22" s="10"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C23" s="10"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="C24" s="10"/>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C25" s="10"/>
       <c r="E25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C26" s="10"/>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13"/>
+      <c r="B27" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13"/>
+      <c r="B28" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="C28" s="10"/>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="C29" s="10"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13"/>
+      <c r="B30" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="C30" s="10"/>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13"/>
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="C31" s="10"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="C32" s="10"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C33" s="10"/>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="C34" s="10"/>
       <c r="E34" s="10"/>
     </row>
@@ -3703,8 +3925,24 @@
       <c r="C591" s="10"/>
       <c r="E591" s="10"/>
     </row>
+    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C592" s="10"/>
+      <c r="E592" s="10"/>
+    </row>
+    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C593" s="10"/>
+      <c r="E593" s="10"/>
+    </row>
+    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C594" s="10"/>
+      <c r="E594" s="10"/>
+    </row>
+    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C595" s="10"/>
+      <c r="E595" s="10"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D591 F2:F591">
+  <conditionalFormatting sqref="D32:D595 F32:F595 D2:D29 F2:F29">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3712,7 +3950,7 @@
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C591 E2:E591">
+  <conditionalFormatting sqref="C32:C595 E32:E595 C2:C29 E2:E29">
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3720,8 +3958,24 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D30:D31 F30:F31">
+    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(ISBLANK(D30),C30="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>AND(ISBLANK(D30),C30="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C31 E30:E31">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C591 E2:E591" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C595 E2:E595" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
add acceptance criteria for saving to wishlist
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t xml:space="preserve">Instructions</t>
   </si>
@@ -688,49 +688,19 @@
     <t xml:space="preserve">**NOT IMPLEMENTED YET** As a Helper, I want to be able to save needs to a wish list so I can revisit needs that I have interest in in the future.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">As a Helper, I want to remove needs from my wish list in case I will not be able to afford them in the future.</t>
-    </r>
+    <t xml:space="preserve">Given I am logged in as a helper, when I click add need to wishlist, my wishlist should be updated with the added need.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given I am viewing my wishlist, when I add the need to my basket, the need should be moved from my wishlist into my basket. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">**NOT IMPLEMENTED YET** As a Helper, I want to remove needs from my wish list in case I will not be able to afford them in the future.</t>
   </si>
   <si>
     <t xml:space="preserve">Given I am logged in as a helper when I click remove on a need in my wishlist then the need will be removed from my wishlist.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">As a Helper, I want to view my wish list so I can see the needs I have saved for purchasing later</t>
-    </r>
+    <t xml:space="preserve">**NOT IMPLEMENTED YET** As a Helper, I want to view my wish list so I can see the needs I have saved for purchasing later</t>
   </si>
   <si>
     <t xml:space="preserve">given that I have items in my wish list when I view my wish list then I expect to see a list of all the needs I have saved for later</t>
@@ -742,25 +712,7 @@
     <t xml:space="preserve">given that I have items in my wish list when I remove an item then I expect that item to be removed from the wish list</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">As a Helper, I would like to filter my searches based on whether or not I’ve viewed them before so I can browse needs I have not seen.</t>
-    </r>
+    <t xml:space="preserve">**NOT IMPLEMENTED YET** As a Helper, I would like to filter my searches based on whether or not I’ve viewed them before so I can browse needs I have not seen.</t>
   </si>
   <si>
     <t xml:space="preserve">given that there are both viewed and unviewed needs when I filter for unviewed needs then I expect to see only needs I have not seen before</t>
@@ -772,25 +724,7 @@
     <t xml:space="preserve">given that I reset the filters when I clear the viewed/unviewed filter then I expect to see all available needs again</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">**NOT IMPLEMENTED YET** </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">As a Helper, I would like to filter my searches by price so I can view needs within my current budget.</t>
-    </r>
+    <t xml:space="preserve">**NOT IMPLEMENTED YET** As a Helper, I would like to filter my searches by price so I can view needs within my current budget.</t>
   </si>
   <si>
     <t xml:space="preserve">given that needs exist with different prices when I filter by a specific price range then I expect to see only the needs within that range</t>
@@ -809,7 +743,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -870,12 +804,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -926,7 +854,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -979,11 +907,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1324,10 +1248,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F595"/>
+  <dimension ref="A1:F596"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.87890625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1608,21 +1532,22 @@
       <c r="A24" s="13" t="s">
         <v>47</v>
       </c>
+      <c r="B24" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="C24" s="10"/>
       <c r="E24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
-        <v>48</v>
-      </c>
+      <c r="A25" s="13"/>
       <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="10"/>
       <c r="E25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+    <row r="26" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1631,10 +1556,12 @@
       <c r="C26" s="10"/>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13"/>
+    <row r="27" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>52</v>
+      </c>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C27" s="10"/>
       <c r="E27" s="10"/>
@@ -1642,25 +1569,25 @@
     <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13"/>
       <c r="B28" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" s="10"/>
       <c r="E28" s="10"/>
     </row>
-    <row r="29" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
-        <v>54</v>
-      </c>
+    <row r="29" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13"/>
       <c r="B29" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="10"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13"/>
+    <row r="30" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="B30" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C30" s="10"/>
       <c r="E30" s="10"/>
@@ -1668,36 +1595,40 @@
     <row r="31" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13"/>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C31" s="10"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
-        <v>58</v>
-      </c>
+    <row r="32" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13"/>
       <c r="B32" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="10"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="B33" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C33" s="10"/>
       <c r="E33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34" s="10"/>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C35" s="10"/>
       <c r="E35" s="10"/>
     </row>
@@ -3941,8 +3872,12 @@
       <c r="C595" s="10"/>
       <c r="E595" s="10"/>
     </row>
+    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C596" s="10"/>
+      <c r="E596" s="10"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D32:D595 F32:F595 D2:D29 F2:F29">
+  <conditionalFormatting sqref="D33:D596 F33:F596 D2:D30 F2:F30">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3950,7 +3885,7 @@
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C595 E32:E595 C2:C29 E2:E29">
+  <conditionalFormatting sqref="C33:C596 E33:E596 C2:C30 E2:E30">
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3958,15 +3893,15 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D31 F30:F31">
+  <conditionalFormatting sqref="D31:D32 F31:F32">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND(ISBLANK(D30),C30="Pass")</formula>
+      <formula>AND(ISBLANK(D31),C31="Pass")</formula>
     </cfRule>
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(ISBLANK(D30),C30="Fail")</formula>
+      <formula>AND(ISBLANK(D31),C31="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31 E30:E31">
+  <conditionalFormatting sqref="C31:C32 E31:E32">
     <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"Pass"</formula>
     </cfRule>
@@ -3975,7 +3910,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C595 E2:E595" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C596 E2:E596" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>